<commit_message>
Webinar and CSV tut
</commit_message>
<xml_diff>
--- a/Webinars/BusinessIntelligence/Webinar/Data/MovieBudget.xlsx
+++ b/Webinars/BusinessIntelligence/Webinar/Data/MovieBudget.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="997">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="1113">
   <si>
     <t>Rank</t>
   </si>
@@ -3007,13 +3007,364 @@
   </si>
   <si>
     <t>From Paris With Love</t>
+  </si>
+  <si>
+    <t>13 Going On 30</t>
+  </si>
+  <si>
+    <t>Breakfast at Tiffany's</t>
+  </si>
+  <si>
+    <t>Crocodile Dundee</t>
+  </si>
+  <si>
+    <t>Crocodile Dundee 2</t>
+  </si>
+  <si>
+    <t>Crocodile Dundee in Los Angeles</t>
+  </si>
+  <si>
+    <t>Death to Smoochy</t>
+  </si>
+  <si>
+    <t>Eternal Sunshine of the Spotless Mind</t>
+  </si>
+  <si>
+    <t>Godzilla 1984: Return of Godzilla</t>
+  </si>
+  <si>
+    <t>Godzilla 1985</t>
+  </si>
+  <si>
+    <t>Godzilla 2000</t>
+  </si>
+  <si>
+    <t>Godzilla Against Mechagodzilla</t>
+  </si>
+  <si>
+    <t>Godzilla and Mothra: The Battle for Earth</t>
+  </si>
+  <si>
+    <t>Godzilla Raids Again</t>
+  </si>
+  <si>
+    <t>Godzilla vs. Biollante</t>
+  </si>
+  <si>
+    <t>Godzilla vs. Destroyah</t>
+  </si>
+  <si>
+    <t>Godzilla vs. Gigan</t>
+  </si>
+  <si>
+    <t>Godzilla vs. Hedorah</t>
+  </si>
+  <si>
+    <t>Godzilla vs. King Chidorah</t>
+  </si>
+  <si>
+    <t>Godzilla Vs. Kong</t>
+  </si>
+  <si>
+    <t>Godzilla vs. Mechagodzilla</t>
+  </si>
+  <si>
+    <t>Godzilla vs. Mechagodzilla II</t>
+  </si>
+  <si>
+    <t>Godzilla vs. Megaguirus</t>
+  </si>
+  <si>
+    <t>Godzilla vs. Megalon</t>
+  </si>
+  <si>
+    <t>Godzilla vs. Space Godzilla</t>
+  </si>
+  <si>
+    <t>Godzilla vs. the Sea Monster</t>
+  </si>
+  <si>
+    <t>Godzilla, Mothra and King Ghidorah: Giant Monsters All-Out Attack</t>
+  </si>
+  <si>
+    <t>Godzilla: King of the Monsters</t>
+  </si>
+  <si>
+    <t>Godzilla: Tokyo S.O.S.</t>
+  </si>
+  <si>
+    <t>Gojira</t>
+  </si>
+  <si>
+    <t>King Kong vs. Godzilla</t>
+  </si>
+  <si>
+    <t>Mothra vs. Godzilla</t>
+  </si>
+  <si>
+    <t>Rifftrax Live: Godzilla</t>
+  </si>
+  <si>
+    <t>Son of Godzilla</t>
+  </si>
+  <si>
+    <t>Terror of Mechagodzilla</t>
+  </si>
+  <si>
+    <t>Shin Godjira</t>
+  </si>
+  <si>
+    <t>Kramer vs. Kramer</t>
+  </si>
+  <si>
+    <t>Manhattan</t>
+  </si>
+  <si>
+    <t>Manhattan Murder Mystery</t>
+  </si>
+  <si>
+    <t>Manhattan Nocturne</t>
+  </si>
+  <si>
+    <t>The Manhattan Project</t>
+  </si>
+  <si>
+    <t>Adrift in Manhattan</t>
+  </si>
+  <si>
+    <t>American Tail: The Treasure of Manhattan Island</t>
+  </si>
+  <si>
+    <t>Friday the 13th Part VIII: Jason Takes Manhattan</t>
+  </si>
+  <si>
+    <t>Great Gatsby: Midnight in Manhattan</t>
+  </si>
+  <si>
+    <t>Little Manhattan</t>
+  </si>
+  <si>
+    <t>Night Falls On Manhattan</t>
+  </si>
+  <si>
+    <t>Tales of Manhattan</t>
+  </si>
+  <si>
+    <t>The Muppets Take Manhattan</t>
+  </si>
+  <si>
+    <t>Requiem for a Dream</t>
+  </si>
+  <si>
+    <t>Saturday Night Fever</t>
+  </si>
+  <si>
+    <t>Sweet and Lowdown</t>
+  </si>
+  <si>
+    <t>Sweet Baby Jesus</t>
+  </si>
+  <si>
+    <t>Sweet Charity</t>
+  </si>
+  <si>
+    <t>Sweet Country</t>
+  </si>
+  <si>
+    <t>Sweet Dreams</t>
+  </si>
+  <si>
+    <t>Sweet Hearts Dance</t>
+  </si>
+  <si>
+    <t>Sweet Home Alabama</t>
+  </si>
+  <si>
+    <t>Sweet Home Carolina</t>
+  </si>
+  <si>
+    <t>Sweet Jane</t>
+  </si>
+  <si>
+    <t>Sweet Karma</t>
+  </si>
+  <si>
+    <t>Sweet Land</t>
+  </si>
+  <si>
+    <t>Sweet Liberty</t>
+  </si>
+  <si>
+    <t>Sweet Lorraine</t>
+  </si>
+  <si>
+    <t>Sweet Nothing</t>
+  </si>
+  <si>
+    <t>Sweet November</t>
+  </si>
+  <si>
+    <t>Sweet Revenge</t>
+  </si>
+  <si>
+    <t>Sweet Sixteen</t>
+  </si>
+  <si>
+    <t>Sweet Sweet Summertime</t>
+  </si>
+  <si>
+    <t>Sweet Sweetback's Baad Asssss Song</t>
+  </si>
+  <si>
+    <t>Sweet Talker</t>
+  </si>
+  <si>
+    <t>Sweet Virginia</t>
+  </si>
+  <si>
+    <t>Sweetgrass</t>
+  </si>
+  <si>
+    <t>Sweethearts</t>
+  </si>
+  <si>
+    <t>Sweethearts of the Gridiron</t>
+  </si>
+  <si>
+    <t>Sweethearts of the Prison Rodeo</t>
+  </si>
+  <si>
+    <t>Sweetheat Deal</t>
+  </si>
+  <si>
+    <t>Sweetiee Weds NRI</t>
+  </si>
+  <si>
+    <t>Sweetwater</t>
+  </si>
+  <si>
+    <t>When a Man Loves a Woman</t>
+  </si>
+  <si>
+    <t>When a Stranger Calls</t>
+  </si>
+  <si>
+    <t>When Brandon Met Trudy</t>
+  </si>
+  <si>
+    <t>When Calls the Heart</t>
+  </si>
+  <si>
+    <t>When Calls the Heart: Healing Heart</t>
+  </si>
+  <si>
+    <t>When Calls The Heart: Heart and Soul</t>
+  </si>
+  <si>
+    <t>When Calls the Heart: The Heart of a Teacher</t>
+  </si>
+  <si>
+    <t>When Calls the Heart: The Heart of Faith</t>
+  </si>
+  <si>
+    <t>When Comedy Went to School</t>
+  </si>
+  <si>
+    <t>When Do We Eat?</t>
+  </si>
+  <si>
+    <t>When Elephants Were Young</t>
+  </si>
+  <si>
+    <t>When Harry Met Sally…</t>
+  </si>
+  <si>
+    <t>When Harry Tries to Marry</t>
+  </si>
+  <si>
+    <t>When I Close My Eyes</t>
+  </si>
+  <si>
+    <t>When I Live My Life Over Again</t>
+  </si>
+  <si>
+    <t>When in Rome</t>
+  </si>
+  <si>
+    <t>When Larry Met Mary</t>
+  </si>
+  <si>
+    <t>When Love Begins...</t>
+  </si>
+  <si>
+    <t>When Love Comes</t>
+  </si>
+  <si>
+    <t>When Love Happens</t>
+  </si>
+  <si>
+    <t>When Love Happens Again</t>
+  </si>
+  <si>
+    <t>When Night is Falling</t>
+  </si>
+  <si>
+    <t>When Shadows Die</t>
+  </si>
+  <si>
+    <t>When Stand Up Stood Out</t>
+  </si>
+  <si>
+    <t>When the Bough Breaks</t>
+  </si>
+  <si>
+    <t>When The Cat's Away</t>
+  </si>
+  <si>
+    <t>When the Checks Stop Coming In</t>
+  </si>
+  <si>
+    <t>When the Game Stands Tall</t>
+  </si>
+  <si>
+    <t>When the Iron Bird Flies</t>
+  </si>
+  <si>
+    <t>When the Road Bends: Tales of a Gypsy Caravan</t>
+  </si>
+  <si>
+    <t>When Time Ran Out...</t>
+  </si>
+  <si>
+    <t>When Two Worlds Collide</t>
+  </si>
+  <si>
+    <t>When We Were Kings</t>
+  </si>
+  <si>
+    <t>When Will I Be Loved</t>
+  </si>
+  <si>
+    <t>When Worlds Collide</t>
+  </si>
+  <si>
+    <t>When You're Strange: A Film About The Doors</t>
+  </si>
+  <si>
+    <t>American Psycho</t>
+  </si>
+  <si>
+    <t>West Side Story</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3021,16 +3372,317 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -3038,16 +3690,208 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3346,10 +4190,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1001"/>
+  <dimension ref="A1:F1125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A1098" workbookViewId="0">
+      <selection activeCell="C720" sqref="C720"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23380,6 +24224,1778 @@
       </c>
       <c r="F1001">
         <v>53139168</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1002" s="3">
+        <v>38100</v>
+      </c>
+      <c r="C1002" s="2" t="s">
+        <v>997</v>
+      </c>
+      <c r="D1002" s="4">
+        <v>37000000</v>
+      </c>
+      <c r="E1002" s="4">
+        <v>57139723</v>
+      </c>
+      <c r="F1002" s="4">
+        <v>97658712</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1003" s="3">
+        <v>22559</v>
+      </c>
+      <c r="C1003" s="2" t="s">
+        <v>998</v>
+      </c>
+      <c r="E1003" s="4">
+        <v>9551904</v>
+      </c>
+      <c r="F1003" s="4">
+        <v>9551904</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1004" s="3">
+        <v>31681</v>
+      </c>
+      <c r="C1004" s="2" t="s">
+        <v>999</v>
+      </c>
+      <c r="D1004" s="4">
+        <v>8800000</v>
+      </c>
+      <c r="E1004" s="4">
+        <v>174803506</v>
+      </c>
+      <c r="F1004" s="4">
+        <v>328203506</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1005" s="3">
+        <v>32288</v>
+      </c>
+      <c r="C1005" s="2" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D1005" s="4">
+        <v>14000000</v>
+      </c>
+      <c r="E1005" s="4">
+        <v>109306210</v>
+      </c>
+      <c r="F1005" s="4">
+        <v>239606210</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1006" s="3">
+        <v>37001</v>
+      </c>
+      <c r="C1006" s="2" t="s">
+        <v>1001</v>
+      </c>
+      <c r="E1006" s="4">
+        <v>25590119</v>
+      </c>
+      <c r="F1006" s="4">
+        <v>39393111</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1007" s="3">
+        <v>37344</v>
+      </c>
+      <c r="C1007" s="2" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D1007" s="4">
+        <v>50000000</v>
+      </c>
+      <c r="E1007" s="4">
+        <v>8355815</v>
+      </c>
+      <c r="F1007" s="4">
+        <v>8374062</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1008" s="3">
+        <v>38065</v>
+      </c>
+      <c r="C1008" s="2" t="s">
+        <v>1003</v>
+      </c>
+      <c r="D1008" s="4">
+        <v>20000000</v>
+      </c>
+      <c r="E1008" s="4">
+        <v>34366518</v>
+      </c>
+      <c r="F1008" s="4">
+        <v>72625689</v>
+      </c>
+    </row>
+    <row r="1009" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1009" s="3">
+        <v>35934</v>
+      </c>
+      <c r="C1009" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1009" s="4">
+        <v>125000000</v>
+      </c>
+      <c r="E1009" s="4">
+        <v>136314294</v>
+      </c>
+      <c r="F1009" s="4">
+        <v>376000000</v>
+      </c>
+    </row>
+    <row r="1010" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1010" s="3">
+        <v>41775</v>
+      </c>
+      <c r="C1010" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1010" s="4">
+        <v>160000000</v>
+      </c>
+      <c r="E1010" s="4">
+        <v>200676069</v>
+      </c>
+      <c r="F1010" s="4">
+        <v>529076069</v>
+      </c>
+    </row>
+    <row r="1011" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1011" s="3">
+        <v>42626</v>
+      </c>
+      <c r="C1011" s="2" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E1011" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1011" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1012" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1012" s="3">
+        <v>31047</v>
+      </c>
+      <c r="C1012" s="2" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E1012" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1012" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1013" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1013" s="3">
+        <v>36756</v>
+      </c>
+      <c r="C1013" s="2" t="s">
+        <v>1006</v>
+      </c>
+      <c r="E1013" s="4">
+        <v>10037390</v>
+      </c>
+      <c r="F1013" s="4">
+        <v>10037390</v>
+      </c>
+    </row>
+    <row r="1014" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1014" s="3">
+        <v>37621</v>
+      </c>
+      <c r="C1014" s="2" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E1014" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1014" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1015" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1015" s="3">
+        <v>33969</v>
+      </c>
+      <c r="C1015" s="2" t="s">
+        <v>1008</v>
+      </c>
+      <c r="E1015" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1015" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1016" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1016" s="3">
+        <v>20454</v>
+      </c>
+      <c r="C1016" s="2" t="s">
+        <v>1009</v>
+      </c>
+      <c r="E1016" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1016" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1017" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1017" s="3">
+        <v>32873</v>
+      </c>
+      <c r="C1017" s="2" t="s">
+        <v>1010</v>
+      </c>
+      <c r="E1017" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1017" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1018" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1018" s="3">
+        <v>35064</v>
+      </c>
+      <c r="C1018" s="2" t="s">
+        <v>1011</v>
+      </c>
+      <c r="E1018" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1018" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1019" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1019" s="3">
+        <v>26664</v>
+      </c>
+      <c r="C1019" s="2" t="s">
+        <v>1012</v>
+      </c>
+      <c r="E1019" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1019" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1020" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1020" s="3">
+        <v>26298</v>
+      </c>
+      <c r="C1020" s="2" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E1020" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1020" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1021" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1021" s="3">
+        <v>33603</v>
+      </c>
+      <c r="C1021" s="2" t="s">
+        <v>1014</v>
+      </c>
+      <c r="E1021" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1021" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1022" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1022" s="3">
+        <v>43973</v>
+      </c>
+      <c r="C1022" s="2" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E1022" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1022" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1023" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1023" s="3">
+        <v>27394</v>
+      </c>
+      <c r="C1023" s="2" t="s">
+        <v>1016</v>
+      </c>
+      <c r="E1023" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1023" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1024" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1024" s="3">
+        <v>34334</v>
+      </c>
+      <c r="C1024" s="2" t="s">
+        <v>1017</v>
+      </c>
+      <c r="E1024" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1024" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1025" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1025" s="3">
+        <v>36891</v>
+      </c>
+      <c r="C1025" s="2" t="s">
+        <v>1018</v>
+      </c>
+      <c r="E1025" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1025" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1026" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1026" s="3">
+        <v>27029</v>
+      </c>
+      <c r="C1026" s="2" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E1026" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1026" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1027" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1027" s="3">
+        <v>34699</v>
+      </c>
+      <c r="C1027" s="2" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E1027" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1027" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1028" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1028" s="3">
+        <v>24472</v>
+      </c>
+      <c r="C1028" s="2" t="s">
+        <v>1021</v>
+      </c>
+      <c r="E1028" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1028" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1029" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1029" s="3">
+        <v>37256</v>
+      </c>
+      <c r="C1029" s="2" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E1029" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1029" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1030" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1030" s="3">
+        <v>20455</v>
+      </c>
+      <c r="C1030" s="2" t="s">
+        <v>1023</v>
+      </c>
+      <c r="E1030" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1030" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1031" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1031" s="3">
+        <v>43546</v>
+      </c>
+      <c r="C1031" s="2" t="s">
+        <v>1023</v>
+      </c>
+      <c r="E1031" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1031" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1032" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1032" s="3">
+        <v>37986</v>
+      </c>
+      <c r="C1032" s="2" t="s">
+        <v>1024</v>
+      </c>
+      <c r="E1032" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1032" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1033" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1033" s="3">
+        <v>41747</v>
+      </c>
+      <c r="C1033" s="2" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E1033" s="4">
+        <v>491389</v>
+      </c>
+      <c r="F1033" s="4">
+        <v>491389</v>
+      </c>
+    </row>
+    <row r="1034" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1034" s="3">
+        <v>31282</v>
+      </c>
+      <c r="C1034" s="2" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E1034" s="4">
+        <v>2443200</v>
+      </c>
+      <c r="F1034" s="4">
+        <v>2443200</v>
+      </c>
+    </row>
+    <row r="1035" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1035" s="3">
+        <v>41730</v>
+      </c>
+      <c r="C1035" s="2" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E1035" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1035" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1036" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1036" s="3">
+        <v>23742</v>
+      </c>
+      <c r="C1036" s="2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E1036" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1036" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1037" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1037" s="3">
+        <v>41865</v>
+      </c>
+      <c r="C1037" s="2" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E1037" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1037" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1038" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1038" s="3">
+        <v>24837</v>
+      </c>
+      <c r="C1038" s="2" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E1038" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1038" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1039" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1039" s="3">
+        <v>27759</v>
+      </c>
+      <c r="C1039" s="2" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E1039" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1039" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1040" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1040" s="3">
+        <v>42654</v>
+      </c>
+      <c r="C1040" s="2" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E1040" s="4">
+        <v>1908028</v>
+      </c>
+      <c r="F1040" s="4">
+        <v>75612484</v>
+      </c>
+    </row>
+    <row r="1041" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1041" s="3">
+        <v>29208</v>
+      </c>
+      <c r="C1041" s="2" t="s">
+        <v>1032</v>
+      </c>
+      <c r="E1041" s="4">
+        <v>106260000</v>
+      </c>
+      <c r="F1041" s="4">
+        <v>106260000</v>
+      </c>
+    </row>
+    <row r="1042" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1042" s="3">
+        <v>28970</v>
+      </c>
+      <c r="C1042" s="2" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E1042" s="4">
+        <v>39946780</v>
+      </c>
+      <c r="F1042" s="4">
+        <v>39946780</v>
+      </c>
+    </row>
+    <row r="1043" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1043" s="3">
+        <v>34199</v>
+      </c>
+      <c r="C1043" s="2" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E1043" s="4">
+        <v>11330911</v>
+      </c>
+      <c r="F1043" s="4">
+        <v>11330911</v>
+      </c>
+    </row>
+    <row r="1044" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1044" s="3">
+        <v>42510</v>
+      </c>
+      <c r="C1044" s="2" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E1044" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1044" s="4">
+        <v>150432</v>
+      </c>
+    </row>
+    <row r="1045" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1045" s="3">
+        <v>31576</v>
+      </c>
+      <c r="C1045" s="2" t="s">
+        <v>1036</v>
+      </c>
+      <c r="E1045" s="4">
+        <v>3900000</v>
+      </c>
+      <c r="F1045" s="4">
+        <v>3900000</v>
+      </c>
+    </row>
+    <row r="1046" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1046" s="3">
+        <v>39346</v>
+      </c>
+      <c r="C1046" s="2" t="s">
+        <v>1037</v>
+      </c>
+      <c r="E1046" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1046" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1047" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1047" s="3">
+        <v>36571</v>
+      </c>
+      <c r="C1047" s="2" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E1047" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1047" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1048" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1048" s="3">
+        <v>32717</v>
+      </c>
+      <c r="C1048" s="2" t="s">
+        <v>1039</v>
+      </c>
+      <c r="E1048" s="4">
+        <v>14343976</v>
+      </c>
+      <c r="F1048" s="4">
+        <v>14343976</v>
+      </c>
+    </row>
+    <row r="1049" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1049" s="3">
+        <v>41401</v>
+      </c>
+      <c r="C1049" s="2" t="s">
+        <v>1040</v>
+      </c>
+      <c r="E1049" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1049" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1050" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1050" s="3">
+        <v>38625</v>
+      </c>
+      <c r="C1050" s="2" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E1050" s="4">
+        <v>385373</v>
+      </c>
+      <c r="F1050" s="4">
+        <v>385373</v>
+      </c>
+    </row>
+    <row r="1051" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1051" s="3">
+        <v>37603</v>
+      </c>
+      <c r="C1051" s="2" t="s">
+        <v>922</v>
+      </c>
+      <c r="E1051" s="4">
+        <v>93932896</v>
+      </c>
+      <c r="F1051" s="4">
+        <v>163838217</v>
+      </c>
+    </row>
+    <row r="1052" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1052" s="3">
+        <v>35566</v>
+      </c>
+      <c r="C1052" s="2" t="s">
+        <v>1042</v>
+      </c>
+      <c r="E1052" s="4">
+        <v>9889670</v>
+      </c>
+      <c r="F1052" s="4">
+        <v>9889670</v>
+      </c>
+    </row>
+    <row r="1053" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1053" s="3">
+        <v>15342</v>
+      </c>
+      <c r="C1053" s="2" t="s">
+        <v>1043</v>
+      </c>
+      <c r="E1053" s="4">
+        <v>5200000</v>
+      </c>
+      <c r="F1053" s="4">
+        <v>5200000</v>
+      </c>
+    </row>
+    <row r="1054" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1054" s="3">
+        <v>30876</v>
+      </c>
+      <c r="C1054" s="2" t="s">
+        <v>1044</v>
+      </c>
+      <c r="E1054" s="4">
+        <v>25534703</v>
+      </c>
+      <c r="F1054" s="4">
+        <v>25534703</v>
+      </c>
+    </row>
+    <row r="1055" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1055" s="3">
+        <v>36805</v>
+      </c>
+      <c r="C1055" s="2" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D1055" s="4">
+        <v>4500000</v>
+      </c>
+      <c r="E1055" s="4">
+        <v>3635482</v>
+      </c>
+      <c r="F1055" s="4">
+        <v>7389233</v>
+      </c>
+    </row>
+    <row r="1056" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1056" s="3">
+        <v>28475</v>
+      </c>
+      <c r="C1056" s="2" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E1056" s="4">
+        <v>139486124</v>
+      </c>
+      <c r="F1056" s="4">
+        <v>282400000</v>
+      </c>
+    </row>
+    <row r="1057" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1057" s="3">
+        <v>36497</v>
+      </c>
+      <c r="C1057" s="2" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E1057" s="4">
+        <v>4196621</v>
+      </c>
+      <c r="F1057" s="4">
+        <v>4196621</v>
+      </c>
+    </row>
+    <row r="1058" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1058" s="3">
+        <v>40908</v>
+      </c>
+      <c r="C1058" s="2" t="s">
+        <v>1048</v>
+      </c>
+      <c r="E1058" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1058" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1059" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1059" s="3">
+        <v>25204</v>
+      </c>
+      <c r="C1059" s="2" t="s">
+        <v>1049</v>
+      </c>
+      <c r="E1059" s="4">
+        <v>8000000</v>
+      </c>
+      <c r="F1059" s="4">
+        <v>8000000</v>
+      </c>
+    </row>
+    <row r="1060" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1060" s="3">
+        <v>43175</v>
+      </c>
+      <c r="C1060" s="2" t="s">
+        <v>1050</v>
+      </c>
+      <c r="E1060" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1060" s="4">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="1061" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1061" s="3">
+        <v>31322</v>
+      </c>
+      <c r="C1061" s="2" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E1061" s="4">
+        <v>9100000</v>
+      </c>
+      <c r="F1061" s="4">
+        <v>9100000</v>
+      </c>
+    </row>
+    <row r="1062" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1062" s="3">
+        <v>41593</v>
+      </c>
+      <c r="C1062" s="2" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E1062" s="4">
+        <v>59403</v>
+      </c>
+      <c r="F1062" s="4">
+        <v>59403</v>
+      </c>
+    </row>
+    <row r="1063" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1063" s="3">
+        <v>32409</v>
+      </c>
+      <c r="C1063" s="2" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E1063" s="4">
+        <v>3790493</v>
+      </c>
+      <c r="F1063" s="4">
+        <v>3790493</v>
+      </c>
+    </row>
+    <row r="1064" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1064" s="3">
+        <v>37526</v>
+      </c>
+      <c r="C1064" s="2" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E1064" s="4">
+        <v>127214072</v>
+      </c>
+      <c r="F1064" s="4">
+        <v>182365114</v>
+      </c>
+    </row>
+    <row r="1065" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1065" s="3">
+        <v>42857</v>
+      </c>
+      <c r="C1065" s="2" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E1065" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1065" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1066" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1066" s="3">
+        <v>36721</v>
+      </c>
+      <c r="C1066" s="2" t="s">
+        <v>1055</v>
+      </c>
+      <c r="E1066" s="4">
+        <v>967</v>
+      </c>
+      <c r="F1066" s="4">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="1067" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1067" s="3">
+        <v>40708</v>
+      </c>
+      <c r="C1067" s="2" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E1067" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1067" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1068" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1068" s="3">
+        <v>39003</v>
+      </c>
+      <c r="C1068" s="2" t="s">
+        <v>1057</v>
+      </c>
+      <c r="E1068" s="4">
+        <v>1706325</v>
+      </c>
+      <c r="F1068" s="4">
+        <v>1706325</v>
+      </c>
+    </row>
+    <row r="1069" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1069" s="3">
+        <v>31546</v>
+      </c>
+      <c r="C1069" s="2" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E1069" s="4">
+        <v>14205021</v>
+      </c>
+      <c r="F1069" s="4">
+        <v>14205021</v>
+      </c>
+    </row>
+    <row r="1070" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1070" s="3">
+        <v>42115</v>
+      </c>
+      <c r="C1070" s="2" t="s">
+        <v>1059</v>
+      </c>
+      <c r="E1070" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1070" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1071" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1071" s="3">
+        <v>35314</v>
+      </c>
+      <c r="C1071" s="2" t="s">
+        <v>1060</v>
+      </c>
+      <c r="E1071" s="4">
+        <v>79249</v>
+      </c>
+      <c r="F1071" s="4">
+        <v>79249</v>
+      </c>
+    </row>
+    <row r="1072" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1072" s="3">
+        <v>36938</v>
+      </c>
+      <c r="C1072" s="2" t="s">
+        <v>1061</v>
+      </c>
+      <c r="E1072" s="4">
+        <v>25288103</v>
+      </c>
+      <c r="F1072" s="4">
+        <v>65754228</v>
+      </c>
+    </row>
+    <row r="1073" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1073" s="3">
+        <v>31777</v>
+      </c>
+      <c r="C1073" s="2" t="s">
+        <v>1062</v>
+      </c>
+      <c r="E1073" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1073" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1074" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1074" s="3">
+        <v>37757</v>
+      </c>
+      <c r="C1074" s="2" t="s">
+        <v>1063</v>
+      </c>
+      <c r="E1074" s="4">
+        <v>304676</v>
+      </c>
+      <c r="F1074" s="4">
+        <v>304676</v>
+      </c>
+    </row>
+    <row r="1075" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1075" s="3">
+        <v>43100</v>
+      </c>
+      <c r="C1075" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E1075" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1075" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1076" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1076" s="3">
+        <v>25934</v>
+      </c>
+      <c r="C1076" s="2" t="s">
+        <v>1065</v>
+      </c>
+      <c r="E1076" s="4">
+        <v>15200000</v>
+      </c>
+      <c r="F1076" s="4">
+        <v>15200000</v>
+      </c>
+    </row>
+    <row r="1077" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1077" s="3">
+        <v>33368</v>
+      </c>
+      <c r="C1077" s="2" t="s">
+        <v>1066</v>
+      </c>
+      <c r="E1077" s="4">
+        <v>258105</v>
+      </c>
+      <c r="F1077" s="4">
+        <v>258105</v>
+      </c>
+    </row>
+    <row r="1078" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1078" s="3">
+        <v>43056</v>
+      </c>
+      <c r="C1078" s="2" t="s">
+        <v>1067</v>
+      </c>
+      <c r="E1078" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1078" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1079" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1079" s="3">
+        <v>40184</v>
+      </c>
+      <c r="C1079" s="2" t="s">
+        <v>1068</v>
+      </c>
+      <c r="E1079" s="4">
+        <v>207473</v>
+      </c>
+      <c r="F1079" s="4">
+        <v>207473</v>
+      </c>
+    </row>
+    <row r="1080" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1080" s="3">
+        <v>13881</v>
+      </c>
+      <c r="C1080" s="2" t="s">
+        <v>1069</v>
+      </c>
+      <c r="E1080" s="4">
+        <v>3000000</v>
+      </c>
+      <c r="F1080" s="4">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="1081" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1081" s="3">
+        <v>42619</v>
+      </c>
+      <c r="C1081" s="2" t="s">
+        <v>1070</v>
+      </c>
+      <c r="E1081" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1081" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1082" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1082" s="3">
+        <v>40438</v>
+      </c>
+      <c r="C1082" s="2" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E1082" s="4">
+        <v>2198</v>
+      </c>
+      <c r="F1082" s="4">
+        <v>2198</v>
+      </c>
+    </row>
+    <row r="1083" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1083" s="3">
+        <v>42735</v>
+      </c>
+      <c r="C1083" s="2" t="s">
+        <v>1072</v>
+      </c>
+      <c r="E1083" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1083" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1084" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1084" s="3">
+        <v>43100</v>
+      </c>
+      <c r="C1084" s="2" t="s">
+        <v>1073</v>
+      </c>
+      <c r="E1084" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1084" s="4">
+        <v>22666</v>
+      </c>
+    </row>
+    <row r="1085" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1085" s="3">
+        <v>41558</v>
+      </c>
+      <c r="C1085" s="2" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E1085" s="4">
+        <v>6147</v>
+      </c>
+      <c r="F1085" s="4">
+        <v>6147</v>
+      </c>
+    </row>
+    <row r="1086" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1086" s="3">
+        <v>34453</v>
+      </c>
+      <c r="C1086" s="2" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E1086" s="4">
+        <v>50021959</v>
+      </c>
+      <c r="F1086" s="4">
+        <v>50021959</v>
+      </c>
+    </row>
+    <row r="1087" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1087" s="3">
+        <v>29126</v>
+      </c>
+      <c r="C1087" s="2" t="s">
+        <v>1076</v>
+      </c>
+      <c r="E1087" s="4">
+        <v>1262052</v>
+      </c>
+      <c r="F1087" s="4">
+        <v>1262052</v>
+      </c>
+    </row>
+    <row r="1088" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1088" s="3">
+        <v>38751</v>
+      </c>
+      <c r="C1088" s="2" t="s">
+        <v>1076</v>
+      </c>
+      <c r="E1088" s="4">
+        <v>47860214</v>
+      </c>
+      <c r="F1088" s="4">
+        <v>67215435</v>
+      </c>
+    </row>
+    <row r="1089" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1089" s="3">
+        <v>36959</v>
+      </c>
+      <c r="C1089" s="2" t="s">
+        <v>1077</v>
+      </c>
+      <c r="E1089" s="4">
+        <v>132384</v>
+      </c>
+      <c r="F1089" s="4">
+        <v>132384</v>
+      </c>
+    </row>
+    <row r="1090" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1090" s="3">
+        <v>41639</v>
+      </c>
+      <c r="C1090" s="2" t="s">
+        <v>1078</v>
+      </c>
+      <c r="E1090" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1090" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1091" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1091" s="3">
+        <v>42983</v>
+      </c>
+      <c r="C1091" s="2" t="s">
+        <v>1079</v>
+      </c>
+      <c r="E1091" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1091" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1092" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1092" s="3">
+        <v>42178</v>
+      </c>
+      <c r="C1092" s="2" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E1092" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1092" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1093" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1093" s="3">
+        <v>42920</v>
+      </c>
+      <c r="C1093" s="2" t="s">
+        <v>1081</v>
+      </c>
+      <c r="E1093" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1093" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1094" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1094" s="3">
+        <v>42815</v>
+      </c>
+      <c r="C1094" s="2" t="s">
+        <v>1082</v>
+      </c>
+      <c r="E1094" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1094" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1095" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1095" s="3">
+        <v>41488</v>
+      </c>
+      <c r="C1095" s="2" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E1095" s="4">
+        <v>365548</v>
+      </c>
+      <c r="F1095" s="4">
+        <v>365548</v>
+      </c>
+    </row>
+    <row r="1096" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1096" s="3">
+        <v>38814</v>
+      </c>
+      <c r="C1096" s="2" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E1096" s="4">
+        <v>431513</v>
+      </c>
+      <c r="F1096" s="4">
+        <v>431513</v>
+      </c>
+    </row>
+    <row r="1097" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1097" s="3">
+        <v>42752</v>
+      </c>
+      <c r="C1097" s="2" t="s">
+        <v>1085</v>
+      </c>
+      <c r="E1097" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1097" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1098" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1098" s="3">
+        <v>32703</v>
+      </c>
+      <c r="C1098" s="2" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D1098" s="4">
+        <v>16000000</v>
+      </c>
+      <c r="E1098" s="4">
+        <v>92823546</v>
+      </c>
+      <c r="F1098" s="4">
+        <v>92961960</v>
+      </c>
+    </row>
+    <row r="1099" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1099" s="3">
+        <v>40655</v>
+      </c>
+      <c r="C1099" s="2" t="s">
+        <v>1087</v>
+      </c>
+      <c r="E1099" s="4">
+        <v>38261</v>
+      </c>
+      <c r="F1099" s="4">
+        <v>38261</v>
+      </c>
+    </row>
+    <row r="1100" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1100" s="3">
+        <v>35986</v>
+      </c>
+      <c r="C1100" s="2" t="s">
+        <v>1088</v>
+      </c>
+      <c r="E1100" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1100" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1101" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1101" s="3">
+        <v>42468</v>
+      </c>
+      <c r="C1101" s="2" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E1101" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1101" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1102" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1102" s="3">
+        <v>40207</v>
+      </c>
+      <c r="C1102" s="2" t="s">
+        <v>1090</v>
+      </c>
+      <c r="E1102" s="4">
+        <v>32680633</v>
+      </c>
+      <c r="F1102" s="4">
+        <v>43796937</v>
+      </c>
+    </row>
+    <row r="1103" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1103" s="3">
+        <v>42735</v>
+      </c>
+      <c r="C1103" s="2" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E1103" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1103" s="4">
+        <v>28751939</v>
+      </c>
+    </row>
+    <row r="1104" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1104" s="3">
+        <v>39813</v>
+      </c>
+      <c r="C1104" s="2" t="s">
+        <v>1092</v>
+      </c>
+      <c r="E1104" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1104" s="4">
+        <v>961448</v>
+      </c>
+    </row>
+    <row r="1105" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1105" s="3">
+        <v>36336</v>
+      </c>
+      <c r="C1105" s="2" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1105" s="4">
+        <v>3242</v>
+      </c>
+      <c r="F1105" s="4">
+        <v>3242</v>
+      </c>
+    </row>
+    <row r="1106" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1106" s="3">
+        <v>42004</v>
+      </c>
+      <c r="C1106" s="2" t="s">
+        <v>1094</v>
+      </c>
+      <c r="E1106" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1106" s="4">
+        <v>7573</v>
+      </c>
+    </row>
+    <row r="1107" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1107" s="3">
+        <v>42735</v>
+      </c>
+      <c r="C1107" s="2" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E1107" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1107" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1108" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1108" s="3">
+        <v>35020</v>
+      </c>
+      <c r="C1108" s="2" t="s">
+        <v>1096</v>
+      </c>
+      <c r="E1108" s="4">
+        <v>919671</v>
+      </c>
+      <c r="F1108" s="4">
+        <v>919671</v>
+      </c>
+    </row>
+    <row r="1109" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1109" s="3">
+        <v>38717</v>
+      </c>
+      <c r="C1109" s="2" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E1109" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1109" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1110" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1110" s="3">
+        <v>38888</v>
+      </c>
+      <c r="C1110" s="2" t="s">
+        <v>1098</v>
+      </c>
+      <c r="E1110" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1110" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1111" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1111" s="3">
+        <v>42622</v>
+      </c>
+      <c r="C1111" s="2" t="s">
+        <v>1099</v>
+      </c>
+      <c r="E1111" s="4">
+        <v>29747603</v>
+      </c>
+      <c r="F1111" s="4">
+        <v>30629507</v>
+      </c>
+    </row>
+    <row r="1112" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1112" s="3">
+        <v>35328</v>
+      </c>
+      <c r="C1112" s="2" t="s">
+        <v>1100</v>
+      </c>
+      <c r="E1112" s="4">
+        <v>1652472</v>
+      </c>
+      <c r="F1112" s="4">
+        <v>2525984</v>
+      </c>
+    </row>
+    <row r="1113" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1113" s="3">
+        <v>42220</v>
+      </c>
+      <c r="C1113" s="2" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E1113" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1113" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1114" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1114" s="3">
+        <v>41873</v>
+      </c>
+      <c r="C1114" s="2" t="s">
+        <v>1102</v>
+      </c>
+      <c r="E1114" s="4">
+        <v>30127963</v>
+      </c>
+      <c r="F1114" s="4">
+        <v>30138912</v>
+      </c>
+    </row>
+    <row r="1115" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1115" s="3">
+        <v>41201</v>
+      </c>
+      <c r="C1115" s="2" t="s">
+        <v>1103</v>
+      </c>
+      <c r="E1115" s="4">
+        <v>13598</v>
+      </c>
+      <c r="F1115" s="4">
+        <v>13598</v>
+      </c>
+    </row>
+    <row r="1116" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1116" s="3">
+        <v>39248</v>
+      </c>
+      <c r="C1116" s="2" t="s">
+        <v>1104</v>
+      </c>
+      <c r="E1116" s="4">
+        <v>442936</v>
+      </c>
+      <c r="F1116" s="4">
+        <v>442936</v>
+      </c>
+    </row>
+    <row r="1117" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1117" s="3">
+        <v>29308</v>
+      </c>
+      <c r="C1117" s="2" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E1117" s="4">
+        <v>3763988</v>
+      </c>
+      <c r="F1117" s="4">
+        <v>3763988</v>
+      </c>
+    </row>
+    <row r="1118" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1118" s="3">
+        <v>42599</v>
+      </c>
+      <c r="C1118" s="2" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E1118" s="4">
+        <v>12080</v>
+      </c>
+      <c r="F1118" s="4">
+        <v>12080</v>
+      </c>
+    </row>
+    <row r="1119" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1119" s="3">
+        <v>35363</v>
+      </c>
+      <c r="C1119" s="2" t="s">
+        <v>1107</v>
+      </c>
+      <c r="E1119" s="4">
+        <v>2666118</v>
+      </c>
+      <c r="F1119" s="4">
+        <v>4647606</v>
+      </c>
+    </row>
+    <row r="1120" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1120" s="3">
+        <v>38240</v>
+      </c>
+      <c r="C1120" s="2" t="s">
+        <v>1108</v>
+      </c>
+      <c r="E1120" s="4">
+        <v>159429</v>
+      </c>
+      <c r="F1120" s="4">
+        <v>159429</v>
+      </c>
+    </row>
+    <row r="1121" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1121" s="3">
+        <v>40908</v>
+      </c>
+      <c r="C1121" s="2" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E1121" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1121" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1122" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1122" s="3">
+        <v>40277</v>
+      </c>
+      <c r="C1122" s="2" t="s">
+        <v>1110</v>
+      </c>
+      <c r="E1122" s="4">
+        <v>246078</v>
+      </c>
+      <c r="F1122" s="4">
+        <v>246078</v>
+      </c>
+    </row>
+    <row r="1123" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1123" s="3">
+        <v>36630</v>
+      </c>
+      <c r="C1123" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D1123" s="4">
+        <v>8000000</v>
+      </c>
+      <c r="E1123" s="4">
+        <v>15070285</v>
+      </c>
+      <c r="F1123" s="4">
+        <v>28674417</v>
+      </c>
+    </row>
+    <row r="1124" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1124" s="3">
+        <v>22572</v>
+      </c>
+      <c r="C1124" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D1124" s="4">
+        <v>6000000</v>
+      </c>
+      <c r="E1124" s="4">
+        <v>43700000</v>
+      </c>
+      <c r="F1124" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1125" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1125" s="3">
+        <v>30841</v>
+      </c>
+      <c r="C1125" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1125" s="4">
+        <v>30000000</v>
+      </c>
+      <c r="E1125" s="4">
+        <v>242212467</v>
+      </c>
+      <c r="F1125" s="4">
+        <v>295212467</v>
       </c>
     </row>
   </sheetData>

</xml_diff>